<commit_message>
fixed the hidden h5 at the carousel
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE5DE6A5-8D3C-4727-B2E1-0704BDFBC6F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="User" sheetId="1" r:id="rId1"/>
+    <sheet name="Roles" sheetId="3" r:id="rId2"/>
+    <sheet name="Projects" sheetId="2" r:id="rId3"/>
+    <sheet name="Task" sheetId="5" r:id="rId4"/>
+    <sheet name="Project status" sheetId="4" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,8 +23,220 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="69">
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Project manager</t>
+  </si>
+  <si>
+    <t>General Manager</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>GM responsible</t>
+  </si>
+  <si>
+    <t>PM responsible</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>deadline</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Id_project</t>
+  </si>
+  <si>
+    <t>Id-project</t>
+  </si>
+  <si>
+    <t>date update</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Jennifer</t>
+  </si>
+  <si>
+    <t>Jessica</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Christopher</t>
+  </si>
+  <si>
+    <t>Matthew</t>
+  </si>
+  <si>
+    <t>Joshua</t>
+  </si>
+  <si>
+    <t>Ashley</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Stephanie</t>
+  </si>
+  <si>
+    <t>Melissa</t>
+  </si>
+  <si>
+    <t>Nicholas</t>
+  </si>
+  <si>
+    <t>Amanda</t>
+  </si>
+  <si>
+    <t>Andrew</t>
+  </si>
+  <si>
+    <t>Brandon</t>
+  </si>
+  <si>
+    <t>Kelly</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Megan</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>Williams</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>Miller</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>Rodriguez</t>
+  </si>
+  <si>
+    <t>Martinez</t>
+  </si>
+  <si>
+    <t>Hernandez</t>
+  </si>
+  <si>
+    <t>Lopez</t>
+  </si>
+  <si>
+    <t>Gonzalez</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>Thomas</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>Moore</t>
+  </si>
+  <si>
+    <t>Jackson</t>
+  </si>
+  <si>
+    <t>Martin</t>
+  </si>
+  <si>
+    <t>Resource</t>
+  </si>
+  <si>
+    <t>Back-end</t>
+  </si>
+  <si>
+    <t>Create a database schema</t>
+  </si>
+  <si>
+    <t>Implement authentication and authorization features</t>
+  </si>
+  <si>
+    <t>Create a server-side application and API</t>
+  </si>
+  <si>
+    <t>Implement security measures</t>
+  </si>
+  <si>
+    <t>Develop landing page</t>
+  </si>
+  <si>
+    <t>Develop contact us page</t>
+  </si>
+  <si>
+    <t>develop login page</t>
+  </si>
+  <si>
+    <t>Front-end</t>
+  </si>
+  <si>
+    <t>Assigned to</t>
+  </si>
+  <si>
+    <t>ongoing</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -49,13 +266,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -66,6 +291,60 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BE3A67D8-4E17-423B-84D1-CD0FAEBFD316}" name="Table1" displayName="Table1" ref="A1:D21" totalsRowShown="0">
+  <autoFilter ref="A1:D21" xr:uid="{F7C106E9-4456-4DB8-9574-FA85467EB9AA}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{3FC81E94-4062-4B9D-BA88-B34FEEA8765F}" name="id"/>
+    <tableColumn id="2" xr3:uid="{04FB2B35-99D6-4BBD-865A-5AE8DA0361DD}" name="Name"/>
+    <tableColumn id="3" xr3:uid="{8C2054C5-221A-47E0-893F-009994AF4C15}" name="Surname"/>
+    <tableColumn id="4" xr3:uid="{BE4D78C8-E582-4D84-A96F-BCC4A57E2672}" name="Role"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{88E444BE-3D6B-4AE6-96C5-891CE705D701}" name="Role" displayName="Role" ref="A1:A4" totalsRowShown="0">
+  <autoFilter ref="A1:A4" xr:uid="{A2064D3F-71C9-4F47-9250-76E20466664A}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{B3061365-ACD7-448B-A7DC-E5298E9D4AA9}" name="Column1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5E15206A-B6A0-4585-B40B-7D18BEE728DB}" name="Table3" displayName="Table3" ref="A1:F8" totalsRowShown="0">
+  <autoFilter ref="A1:F8" xr:uid="{F9F297AD-55F0-4804-9311-769C923B9131}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{BF8FF2D6-D9E2-4635-B5D4-CC9DC301CC07}" name="id"/>
+    <tableColumn id="2" xr3:uid="{23986541-87B2-4B51-9A54-10B0EBB263C2}" name="Name"/>
+    <tableColumn id="3" xr3:uid="{C1E4D933-EF49-4BBA-898B-808F89078DDE}" name="Category"/>
+    <tableColumn id="4" xr3:uid="{93FBD156-E2AB-4CE7-9406-ED150651CD31}" name="GM responsible"/>
+    <tableColumn id="5" xr3:uid="{068BEF5B-D437-4EA7-8BA1-B1D30956DA04}" name="PM responsible"/>
+    <tableColumn id="6" xr3:uid="{83BBA40F-0F96-4EF8-AB86-2CB12EBD3A14}" name="deadline"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{31A6874D-9BED-44C3-952E-83B61F6AF261}" name="Table4" displayName="Table4" ref="A1:G11" totalsRowShown="0">
+  <autoFilter ref="A1:G11" xr:uid="{AED6A908-0C65-4C22-8428-20D0D5ADC447}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{C38F0B36-8084-43B0-9B1F-1E977023E492}" name="id"/>
+    <tableColumn id="2" xr3:uid="{6D6E1DC0-EB5E-4A5C-AE00-39D0D69EB34D}" name="Id_project"/>
+    <tableColumn id="3" xr3:uid="{3FDD2822-2F4D-4936-BABE-A8A2ABD66EFF}" name="Assigned to"/>
+    <tableColumn id="4" xr3:uid="{A458EA19-76C4-45EA-B886-30CDB9B52F8B}" name="Name"/>
+    <tableColumn id="5" xr3:uid="{344D4A63-DB9D-4FA6-B168-7612DE209137}" name="deadline" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{0CD63EEA-8477-43F5-8D65-369D6DAF9628}" name="status"/>
+    <tableColumn id="7" xr3:uid="{50C7ABD0-1330-466B-BF30-E8717E731763}" name="remarks"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,13 +609,848 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <f>1+A2</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <f t="shared" ref="A4:A21" si="0">1+A3</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" s="1"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="s">
+        <v>4</v>
+      </c>
+      <c r="J11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
+        <v>57</v>
+      </c>
+      <c r="J13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" s="1"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" s="1"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+      <c r="J17" s="1"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" s="1"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" t="s">
+        <v>57</v>
+      </c>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="J20" s="1"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1EE0A2F7-2DF4-4787-8F51-9797B63FD73A}">
+          <x14:formula1>
+            <xm:f>Roles!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>D2:D21</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84F66F99-B9ED-4AC0-B61C-78D4F70B59A1}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="18.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18ADD3EB-0303-4595-B7BA-E11D303E7B56}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2">
+        <v>45008</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45009</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45010</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45011</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45012</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2">
+        <v>45013</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2">
+        <v>45014</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{935484C7-0CBE-46E0-AB93-A3CF9508F53F}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="3" width="17.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2">
+        <v>44979</v>
+      </c>
+      <c r="F2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>15</v>
+      </c>
+      <c r="E3" s="2">
+        <v>44980</v>
+      </c>
+      <c r="F3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2">
+        <v>44981</v>
+      </c>
+      <c r="F4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2">
+        <v>44982</v>
+      </c>
+      <c r="F5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>14</v>
+      </c>
+      <c r="E6" s="2">
+        <v>44983</v>
+      </c>
+      <c r="F6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>14</v>
+      </c>
+      <c r="E7" s="2">
+        <v>44984</v>
+      </c>
+      <c r="F7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>44985</v>
+      </c>
+      <c r="F8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="2">
+        <v>44986</v>
+      </c>
+      <c r="F9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="2">
+        <v>44987</v>
+      </c>
+      <c r="F10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="2">
+        <v>44988</v>
+      </c>
+      <c r="F11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC7AF7A-CC4A-4FCC-B755-03726C695879}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>